<commit_message>
Newest code tested and built, new pin num sheet
Adapted begin.vi and set this code as startup as of 02/17/13. Fixed
missing negative signs in teleop for certain axis. Set begin.vi
motor/solenoid/relay openings correctly. Updated pin num sheet
accordingly.
</commit_message>
<xml_diff>
--- a/Documents/Pin Numbers 02-16-13.xlsx
+++ b/Documents/Pin Numbers 02-16-13.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="19320" windowHeight="12120"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="19320" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -168,8 +168,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +304,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -338,6 +339,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -513,14 +515,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
@@ -530,7 +532,7 @@
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -550,7 +552,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -570,7 +572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -587,7 +589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -597,14 +599,11 @@
       <c r="E4">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
       <c r="H4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -621,7 +620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -631,11 +630,14 @@
       <c r="E6">
         <v>5</v>
       </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
       <c r="H6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -649,7 +651,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -663,7 +665,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -677,7 +679,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -691,7 +693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -705,7 +707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -719,7 +721,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -736,7 +738,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -753,10 +755,10 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -773,10 +775,10 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -793,10 +795,10 @@
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -813,40 +815,40 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E18">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E19">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E20">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E21">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E25">
         <v>2</v>
       </c>
@@ -854,7 +856,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E26">
         <v>3</v>
       </c>
@@ -862,12 +864,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E27">
         <v>4</v>
       </c>
       <c r="F27" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -878,24 +880,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>